<commit_message>
Waitlist Api is now working and Logo Issue is also fixed
</commit_message>
<xml_diff>
--- a/survey_responses.xlsx
+++ b/survey_responses.xlsx
@@ -1,83 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAMARTH SNEH\Desktop\Mithi files\freelance\Pettxo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F05642D-2AC0-4EAD-9CA0-7C69070FE61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Responses" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t>Do you currently own a pet?</t>
-  </si>
-  <si>
-    <t>What breed(s) is your pet? (optional)</t>
-  </si>
-  <si>
-    <t>How long have you had your pet?</t>
-  </si>
-  <si>
-    <t>What is your primary concern when it comes to pet care? (Select up to 3)</t>
-  </si>
-  <si>
-    <t>How do you currently meet your pet's needs in these areas?</t>
-  </si>
-  <si>
-    <t>What features would you find most useful in a pet care app? (Select up to 3)</t>
-  </si>
-  <si>
-    <t>How likely are you to use an app like Pettxo if it offered the features you need?</t>
-  </si>
-  <si>
-    <t>Do you have any other comments or suggestions for us?</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Bird, Fish, Rabbit</t>
-  </si>
-  <si>
-    <t>cat</t>
-  </si>
-  <si>
-    <t>less_than_a_year</t>
-  </si>
-  <si>
-    <t>Nutrition</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>Appointment scheduling</t>
-  </si>
-  <si>
-    <t>very_likely</t>
-  </si>
-  <si>
-    <t>bh</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,21 +65,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -446,87 +396,201 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="25.09765625" customWidth="1"/>
-    <col min="2" max="2" width="25.296875" customWidth="1"/>
-    <col min="3" max="3" width="31.69921875" customWidth="1"/>
-    <col min="4" max="4" width="28.8984375" customWidth="1"/>
-    <col min="5" max="5" width="63.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.69921875" customWidth="1"/>
-    <col min="7" max="7" width="64.796875" customWidth="1"/>
-    <col min="8" max="8" width="67.5" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>First Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Last Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Email Confirm</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Location</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Do you currently own a pet?</v>
+      </c>
+      <c r="G1" t="str">
+        <v>What type(s) of pet do you have?</v>
+      </c>
+      <c r="H1" t="str">
+        <v>What breed(s) is your pet?</v>
+      </c>
+      <c r="I1" t="str">
+        <v>What is the gender of your pet?</v>
+      </c>
+      <c r="J1" t="str">
+        <v>What is your biggest challenge with pet care?</v>
+      </c>
+      <c r="K1" t="str">
+        <v>When do you plan to get a pet?</v>
+      </c>
+      <c r="L1" t="str">
+        <v>What type of pet are you interested in?</v>
+      </c>
+      <c r="M1" t="str">
+        <v>What is your primary concern when it comes to pet care?</v>
+      </c>
+      <c r="N1" t="str">
+        <v>What type of pet-related service do you offer?</v>
+      </c>
+      <c r="O1" t="str">
+        <v>What specific services do you provide?</v>
+      </c>
+      <c r="P1" t="str">
+        <v>What apps or platforms do you currently use?</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>How often would you like to receive content?</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Which platform(s) are you interested in?</v>
+      </c>
+      <c r="S1" t="str">
+        <v>How likely are you to use Pettxo?</v>
+      </c>
+      <c r="T1" t="str">
+        <v>What features would you find useful?</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>aus</v>
+      </c>
+      <c r="B2" t="str">
+        <v/>
+      </c>
+      <c r="C2" t="str">
+        <v>asusred730@gmail.com</v>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v>Benguluru</v>
+      </c>
+      <c r="F2" t="str">
+        <v>DOG</v>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <v/>
+      </c>
+      <c r="M2" t="str">
+        <v/>
+      </c>
+      <c r="N2" t="str">
+        <v/>
+      </c>
+      <c r="O2" t="str">
+        <v/>
+      </c>
+      <c r="P2" t="str">
+        <v/>
+      </c>
+      <c r="Q2" t="str">
+        <v/>
+      </c>
+      <c r="R2" t="str">
+        <v/>
+      </c>
+      <c r="S2" t="str">
+        <v/>
+      </c>
+      <c r="T2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>ausuuu</v>
+      </c>
+      <c r="B3" t="str">
+        <v/>
+      </c>
+      <c r="C3" t="str">
+        <v>asusred730@gmail.com</v>
+      </c>
+      <c r="D3" t="str">
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <v>Benguluru</v>
+      </c>
+      <c r="F3" t="str">
+        <v>DOG</v>
+      </c>
+      <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <v/>
+      </c>
+      <c r="I3" t="str">
+        <v/>
+      </c>
+      <c r="J3" t="str">
+        <v/>
+      </c>
+      <c r="K3" t="str">
+        <v/>
+      </c>
+      <c r="L3" t="str">
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3" t="str">
+        <v/>
+      </c>
+      <c r="O3" t="str">
+        <v/>
+      </c>
+      <c r="P3" t="str">
+        <v/>
+      </c>
+      <c r="Q3" t="str">
+        <v/>
+      </c>
+      <c r="R3" t="str">
+        <v/>
+      </c>
+      <c r="S3" t="str">
+        <v/>
+      </c>
+      <c r="T3" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:I2 A1 C1:I1" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:T3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>